<commit_message>
error with stable peak fits
</commit_message>
<xml_diff>
--- a/docs/Examples/Example1a_Gas_Cell_Calibration/Calibration_fitting.xlsx
+++ b/docs/Examples/Example1a_Gas_Cell_Calibration/Calibration_fitting.xlsx
@@ -364,7 +364,7 @@
     <t>Flagged Warnings:</t>
   </si>
   <si>
-    <t>Flagged Warnings: HB1_LowSigma HB1_HighAmp</t>
+    <t>Flagged Warnings: No Error</t>
   </si>
   <si>
     <t>POC51</t>
@@ -1419,91 +1419,97 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>102.8029721176377</v>
+        <v>102.8027442038182</v>
       </c>
       <c r="D2">
-        <v>102.8034022310142</v>
+        <v>102.8116901271603</v>
       </c>
       <c r="E2">
-        <v>102.8025420042613</v>
+        <v>102.7937982804761</v>
       </c>
       <c r="F2" t="s">
         <v>57</v>
       </c>
       <c r="G2">
-        <v>102.74028133866</v>
+        <v>102.7400535638137</v>
+      </c>
+      <c r="H2">
+        <v>0.012279461555679</v>
+      </c>
+      <c r="I2">
+        <v>0.008683886320934935</v>
       </c>
       <c r="J2">
-        <v>1286.697274484526</v>
+        <v>1286.697275506042</v>
+      </c>
+      <c r="K2">
+        <v>0.006046742643592262</v>
       </c>
       <c r="L2">
-        <v>179.7541085179101</v>
+        <v>179.7541288309286</v>
       </c>
       <c r="M2">
-        <v>1286.697274484526</v>
+        <v>1286.697275506042</v>
       </c>
       <c r="N2">
-        <v>235.0843298804039</v>
+        <v>235.0844764676349</v>
       </c>
       <c r="O2">
-        <v>0.6143021487950119</v>
+        <v>0.6143020373870589</v>
       </c>
       <c r="P2">
-        <v>3.138012664994625</v>
+        <v>3.138012966572981</v>
       </c>
       <c r="Q2">
-        <v>4.381082892468413E-06</v>
+        <v>6.527587780913446E-06</v>
       </c>
       <c r="R2">
-        <v>1.228604297590024</v>
+        <v>1.228604074774118</v>
       </c>
       <c r="S2" t="s">
         <v>115</v>
       </c>
       <c r="T2">
-        <v>1389.437555823186</v>
+        <v>1389.437329069856</v>
+      </c>
+      <c r="U2">
+        <v>0.006232718912086743</v>
       </c>
       <c r="V2">
-        <v>289.4246075102411</v>
+        <v>290.006191203727</v>
       </c>
       <c r="W2">
-        <v>1389.437555823186</v>
+        <v>1389.437329069856</v>
       </c>
       <c r="X2">
-        <v>375.413972933329</v>
+        <v>379.3411626090142</v>
       </c>
       <c r="Y2">
-        <v>0.5832480321961968</v>
+        <v>0.5816713640334403</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
       </c>
       <c r="AA2">
-        <v>2.388080335394699</v>
+        <v>2.686882185178654</v>
       </c>
       <c r="AB2">
-        <v>0.1325207501273606</v>
+        <v>0.1620861707008304</v>
       </c>
       <c r="AC2">
-        <v>1.166496064392394</v>
+        <v>1.163342728066881</v>
       </c>
       <c r="AD2" t="s">
         <v>115</v>
       </c>
       <c r="AE2">
-        <v>1266.354250392434</v>
+        <v>1266.354250388924</v>
       </c>
       <c r="AF2">
-        <v>15.73253961036479</v>
+        <v>15.73254021978991</v>
       </c>
       <c r="AG2">
-        <v>0.4902690788938933</v>
-      </c>
-      <c r="AH2">
-        <v>1410.662565471161</v>
-      </c>
-      <c r="AI2">
-        <v>27.73682632238576</v>
-      </c>
-      <c r="AJ2">
-        <v>0.5231160349698125</v>
+        <v>0.4902690603456354</v>
       </c>
       <c r="AT2" t="s">
         <v>117</v>
@@ -1550,85 +1556,88 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>102.7968457587915</v>
+        <v>102.7967797671247</v>
       </c>
       <c r="D3">
-        <v>102.8056659066114</v>
+        <v>102.8076899891196</v>
       </c>
       <c r="E3">
-        <v>102.7880256109715</v>
+        <v>102.7858695451298</v>
       </c>
       <c r="F3" t="s">
         <v>58</v>
       </c>
       <c r="G3">
-        <v>102.7342501215824</v>
+        <v>102.7341841700854</v>
+      </c>
+      <c r="H3">
+        <v>0.01489178893835922</v>
+      </c>
+      <c r="I3">
+        <v>0.01069378376823456</v>
       </c>
       <c r="J3">
-        <v>1286.689829391017</v>
+        <v>1286.689828647406</v>
       </c>
       <c r="K3">
-        <v>0.008800000000000001</v>
+        <v>0.008763908579392018</v>
       </c>
       <c r="L3">
-        <v>244.7406157325909</v>
+        <v>244.7405949832576</v>
       </c>
       <c r="M3">
-        <v>1286.689829391017</v>
+        <v>1286.689828647406</v>
       </c>
       <c r="N3">
-        <v>311.318737851742</v>
+        <v>311.3188451094823</v>
       </c>
       <c r="O3">
-        <v>0.5960540565537429</v>
+        <v>0.5960543106132401</v>
       </c>
       <c r="P3">
-        <v>3.751446937461491</v>
+        <v>3.751446303086947</v>
       </c>
       <c r="Q3">
-        <v>4.752461202350844E-10</v>
+        <v>1.754782930074583E-09</v>
       </c>
       <c r="R3">
-        <v>1.192108113107486</v>
+        <v>1.19210862122648</v>
       </c>
       <c r="S3" t="s">
         <v>115</v>
       </c>
       <c r="T3">
-        <v>1389.4240795126</v>
+        <v>1389.424012817491</v>
+      </c>
+      <c r="U3">
+        <v>0.006127880358967198</v>
       </c>
       <c r="V3">
-        <v>384.6821077008112</v>
+        <v>385.1044144990192</v>
       </c>
       <c r="W3">
-        <v>1389.4240795126</v>
+        <v>1389.424012817491</v>
       </c>
       <c r="X3">
-        <v>488.5773488707997</v>
+        <v>491.3372303967248</v>
       </c>
       <c r="Y3">
-        <v>0.5863470122268218</v>
+        <v>0.5854443127621647</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
       </c>
       <c r="AA3">
-        <v>2.588541514345134</v>
+        <v>3.092547136975868</v>
       </c>
       <c r="AB3">
-        <v>0.05321646323705448</v>
+        <v>0.07013379742628134</v>
       </c>
       <c r="AC3">
-        <v>1.172694024453644</v>
+        <v>1.170888625524329</v>
       </c>
       <c r="AD3" t="s">
         <v>115</v>
-      </c>
-      <c r="AH3">
-        <v>1410.673868916109</v>
-      </c>
-      <c r="AI3">
-        <v>40.13701710380058</v>
-      </c>
-      <c r="AJ3">
-        <v>0.5632530031482178</v>
       </c>
       <c r="AT3" t="s">
         <v>118</v>
@@ -1675,91 +1684,97 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>102.8233390973659</v>
+        <v>102.823328086362</v>
       </c>
       <c r="D4">
-        <v>102.8238657148227</v>
+        <v>102.8269921494093</v>
       </c>
       <c r="E4">
-        <v>102.8228124799091</v>
+        <v>102.8196640233147</v>
       </c>
       <c r="F4" t="s">
         <v>59</v>
       </c>
       <c r="G4">
-        <v>102.760787536266</v>
+        <v>102.7607765319449</v>
+      </c>
+      <c r="H4">
+        <v>0.002978303392156865</v>
+      </c>
+      <c r="I4">
+        <v>0.002978303392156865</v>
       </c>
       <c r="J4">
-        <v>1286.67537639385</v>
+        <v>1286.675380917213</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
       </c>
       <c r="L4">
-        <v>219.4474478349248</v>
+        <v>219.9336749782716</v>
       </c>
       <c r="M4">
-        <v>1286.67537639385</v>
+        <v>1286.675380917213</v>
       </c>
       <c r="N4">
-        <v>282.3569888682109</v>
+        <v>287.0962389048356</v>
       </c>
       <c r="O4">
-        <v>0.6043690226795304</v>
+        <v>0.6033008331943694</v>
       </c>
       <c r="P4">
-        <v>2.948797367900801</v>
+        <v>3.065414054505084</v>
       </c>
       <c r="Q4">
-        <v>2.573991473980852E-05</v>
+        <v>0.04203610722108919</v>
       </c>
       <c r="R4">
-        <v>1.208738045359061</v>
+        <v>1.206601666388739</v>
       </c>
       <c r="S4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="T4">
-        <v>1389.436163930116</v>
+        <v>1389.436157449158</v>
+      </c>
+      <c r="U4">
+        <v>0.002978303392156865</v>
       </c>
       <c r="V4">
-        <v>347.8871805667172</v>
+        <v>347.8887883033174</v>
       </c>
       <c r="W4">
-        <v>1389.436163930116</v>
+        <v>1389.436157449158</v>
       </c>
       <c r="X4">
-        <v>437.7333322961238</v>
+        <v>437.7398423560691</v>
       </c>
       <c r="Y4">
-        <v>0.5849230651942121</v>
+        <v>0.5849182516501219</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
       </c>
       <c r="AA4">
-        <v>2.908566136203752</v>
+        <v>2.908524365767789</v>
       </c>
       <c r="AB4">
-        <v>0.03205152865066385</v>
+        <v>0.03210826693627733</v>
       </c>
       <c r="AC4">
-        <v>1.169846130388424</v>
+        <v>1.169836503300244</v>
       </c>
       <c r="AD4" t="s">
         <v>115</v>
       </c>
-      <c r="AE4">
-        <v>1266.533833906227</v>
-      </c>
-      <c r="AF4">
-        <v>17.07576932718324</v>
-      </c>
-      <c r="AG4">
-        <v>0.3739635671801887</v>
-      </c>
       <c r="AH4">
-        <v>1410.546170629767</v>
+        <v>1410.546170618303</v>
       </c>
       <c r="AI4">
-        <v>35.32939876182051</v>
+        <v>35.329373001608</v>
       </c>
       <c r="AJ4">
-        <v>0.4978470048001869</v>
+        <v>0.4978467489414233</v>
       </c>
       <c r="AT4" t="s">
         <v>119</v>
@@ -1806,91 +1821,106 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>102.8218218384112</v>
+        <v>102.8218225229832</v>
       </c>
       <c r="D5">
-        <v>102.8223622031779</v>
+        <v>102.8308485115728</v>
       </c>
       <c r="E5">
-        <v>102.8212814736444</v>
+        <v>102.8127965343937</v>
       </c>
       <c r="F5" t="s">
         <v>60</v>
       </c>
       <c r="G5">
-        <v>102.759339140453</v>
+        <v>102.759339824592</v>
+      </c>
+      <c r="H5">
+        <v>0.01132346262347602</v>
+      </c>
+      <c r="I5">
+        <v>0.008765006006579866</v>
       </c>
       <c r="J5">
-        <v>1286.683841246617</v>
+        <v>1286.683837432701</v>
+      </c>
+      <c r="K5">
+        <v>0.008183132450267132</v>
       </c>
       <c r="L5">
-        <v>183.6164527259793</v>
+        <v>183.6164970473465</v>
       </c>
       <c r="M5">
-        <v>1286.683841246617</v>
+        <v>1286.683837432701</v>
       </c>
       <c r="N5">
-        <v>240.6090760932128</v>
+        <v>240.6091196850258</v>
       </c>
       <c r="O5">
-        <v>0.6155141153018872</v>
+        <v>0.6155138442406235</v>
       </c>
       <c r="P5">
-        <v>3.07169820709617</v>
+        <v>3.071700865154769</v>
       </c>
       <c r="Q5">
-        <v>1.341361802575936E-06</v>
+        <v>2.520785401971537E-06</v>
       </c>
       <c r="R5">
-        <v>1.231028230603774</v>
+        <v>1.231027688481247</v>
       </c>
       <c r="S5" t="s">
         <v>115</v>
       </c>
       <c r="T5">
-        <v>1389.44318038707</v>
+        <v>1389.443227259793</v>
+      </c>
+      <c r="U5">
+        <v>0.003140330173208889</v>
       </c>
       <c r="V5">
-        <v>302.1487620445769</v>
+        <v>302.1507598415413</v>
       </c>
       <c r="W5">
-        <v>1389.44318038707</v>
+        <v>1389.443177257293</v>
       </c>
       <c r="X5">
-        <v>374.1899409801232</v>
+        <v>374.1738743289091</v>
       </c>
       <c r="Y5">
-        <v>0.5817132927133599</v>
+        <v>0.5816960636650494</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
       </c>
       <c r="AA5">
-        <v>3.118956508404149</v>
+        <v>3.196005289867535</v>
       </c>
       <c r="AB5">
-        <v>6.667862646470013E-07</v>
+        <v>1.28774279017918E-08</v>
       </c>
       <c r="AC5">
-        <v>1.16342658542672</v>
+        <v>1.163392127330099</v>
       </c>
       <c r="AD5" t="s">
         <v>115</v>
       </c>
       <c r="AE5">
-        <v>1266.373141341996</v>
+        <v>1266.373141335894</v>
       </c>
       <c r="AF5">
-        <v>19.20339793568952</v>
+        <v>19.20339722595636</v>
       </c>
       <c r="AG5">
-        <v>0.5751141163809599</v>
+        <v>0.5751140545496863</v>
       </c>
       <c r="AH5">
-        <v>1410.651508712812</v>
+        <v>1410.627181908422</v>
       </c>
       <c r="AI5">
-        <v>34.2937202628027</v>
+        <v>42.16060873693058</v>
       </c>
       <c r="AJ5">
-        <v>0.5690067392665132</v>
+        <v>0.1992712256593459</v>
       </c>
       <c r="AT5" t="s">
         <v>120</v>
@@ -1937,91 +1967,88 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>102.7898254356601</v>
+        <v>102.7902111209565</v>
       </c>
       <c r="D6">
-        <v>102.7904056027239</v>
+        <v>102.8047292360994</v>
       </c>
       <c r="E6">
-        <v>102.7892452685963</v>
+        <v>102.7756930058136</v>
       </c>
       <c r="F6" t="s">
         <v>61</v>
       </c>
       <c r="G6">
-        <v>102.7274352336294</v>
+        <v>102.7278206848084</v>
+      </c>
+      <c r="H6">
+        <v>0.01951959861319457</v>
+      </c>
+      <c r="I6">
+        <v>0.01435175972674143</v>
       </c>
       <c r="J6">
-        <v>1286.707956447115</v>
+        <v>1286.707651143</v>
+      </c>
+      <c r="K6">
+        <v>0.01254059435873648</v>
       </c>
       <c r="L6">
-        <v>156.3397980495265</v>
+        <v>156.0745342173684</v>
       </c>
       <c r="M6">
-        <v>1286.707956447115</v>
+        <v>1286.707651143</v>
       </c>
       <c r="N6">
-        <v>206.275458025829</v>
+        <v>208.5880239143283</v>
       </c>
       <c r="O6">
-        <v>0.6197489586579122</v>
+        <v>0.6245138943869486</v>
       </c>
       <c r="P6">
-        <v>3.257016826506569</v>
+        <v>3.075344287110709</v>
       </c>
       <c r="Q6">
-        <v>5.551115123125783E-17</v>
+        <v>2.533084852984757E-12</v>
       </c>
       <c r="R6">
-        <v>1.239497917315824</v>
+        <v>1.249027788773897</v>
       </c>
       <c r="S6" t="s">
         <v>115</v>
       </c>
       <c r="T6">
-        <v>1389.435391680745</v>
+        <v>1389.435471827808</v>
+      </c>
+      <c r="U6">
+        <v>0.00697900425445809</v>
       </c>
       <c r="V6">
-        <v>263.9643198560204</v>
+        <v>263.7608375111804</v>
       </c>
       <c r="W6">
-        <v>1389.435391680745</v>
+        <v>1389.435471827808</v>
       </c>
       <c r="X6">
-        <v>320.7398046133422</v>
+        <v>322.3103659786261</v>
       </c>
       <c r="Y6">
-        <v>0.5707492115237606</v>
+        <v>0.5726887961043112</v>
+      </c>
+      <c r="Z6">
+        <v>0</v>
       </c>
       <c r="AA6">
-        <v>2.859710756010758</v>
+        <v>2.942496238938431</v>
       </c>
       <c r="AB6">
-        <v>7.491157228423084E-07</v>
+        <v>6.568381893945485E-08</v>
       </c>
       <c r="AC6">
-        <v>1.141498423047521</v>
+        <v>1.145377592208622</v>
       </c>
       <c r="AD6" t="s">
         <v>115</v>
-      </c>
-      <c r="AE6">
-        <v>1266.551359020218</v>
-      </c>
-      <c r="AF6">
-        <v>11.73594367537412</v>
-      </c>
-      <c r="AG6">
-        <v>0.5452405583735599</v>
-      </c>
-      <c r="AH6">
-        <v>1410.700525424186</v>
-      </c>
-      <c r="AI6">
-        <v>22.17094744279638</v>
-      </c>
-      <c r="AJ6">
-        <v>0.6027039121659933</v>
       </c>
       <c r="AT6" t="s">
         <v>61</v>
@@ -2068,94 +2095,97 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>102.792116370239</v>
+        <v>102.7919737441313</v>
       </c>
       <c r="D7">
-        <v>102.7982214918648</v>
+        <v>102.8077191928087</v>
       </c>
       <c r="E7">
-        <v>102.7860112486133</v>
+        <v>102.776228295454</v>
       </c>
       <c r="F7" t="s">
         <v>62</v>
       </c>
       <c r="G7">
-        <v>102.7298052377839</v>
+        <v>102.7296626981142</v>
+      </c>
+      <c r="H7">
+        <v>0.01891010925144206</v>
+      </c>
+      <c r="I7">
+        <v>0.01559057432361063</v>
       </c>
       <c r="J7">
-        <v>1286.713955849104</v>
+        <v>1286.714117859994</v>
+      </c>
+      <c r="K7">
+        <v>0.01512382397141193</v>
       </c>
       <c r="L7">
-        <v>131.0450363498051</v>
+        <v>130.8125811186033</v>
       </c>
       <c r="M7">
-        <v>1286.714005851604</v>
+        <v>1286.714117859994</v>
       </c>
       <c r="N7">
-        <v>171.4739003427869</v>
+        <v>173.7138312181267</v>
       </c>
       <c r="O7">
-        <v>0.6146321057309264</v>
+        <v>0.6199414396133358</v>
       </c>
       <c r="P7">
-        <v>3.105422407102474</v>
+        <v>2.919465740733076</v>
       </c>
       <c r="Q7">
-        <v>5.813018177924789E-09</v>
+        <v>6.42167985454023E-11</v>
       </c>
       <c r="R7">
-        <v>1.229264211461853</v>
+        <v>1.239882879226672</v>
       </c>
       <c r="S7" t="s">
         <v>115</v>
       </c>
       <c r="T7">
-        <v>1389.443811089388</v>
+        <v>1389.443780558108</v>
       </c>
       <c r="U7">
-        <v>0.00607</v>
+        <v>0.003786285280030128</v>
       </c>
       <c r="V7">
-        <v>235.0956129133607</v>
+        <v>235.099830632959</v>
       </c>
       <c r="W7">
-        <v>1389.443811089388</v>
+        <v>1389.443780558108</v>
       </c>
       <c r="X7">
-        <v>289.8139099591037</v>
+        <v>289.8211297001717</v>
       </c>
       <c r="Y7">
-        <v>0.5165366818131636</v>
+        <v>0.5165213034276208</v>
+      </c>
+      <c r="Z7">
+        <v>0</v>
       </c>
       <c r="AA7">
-        <v>2.608018924124824</v>
+        <v>2.608060848345964</v>
       </c>
       <c r="AB7">
-        <v>0.3348989353482602</v>
+        <v>0.3350006185512883</v>
       </c>
       <c r="AC7">
-        <v>1.033073363626327</v>
+        <v>1.033042606855242</v>
       </c>
       <c r="AD7" t="s">
         <v>115</v>
       </c>
-      <c r="AE7">
-        <v>1266.571750547651</v>
-      </c>
-      <c r="AF7">
-        <v>26.24523377974807</v>
-      </c>
-      <c r="AG7">
-        <v>0.1564675051017412</v>
-      </c>
       <c r="AH7">
-        <v>1410.669148494898</v>
+        <v>1410.669144030468</v>
       </c>
       <c r="AI7">
-        <v>23.11251176129749</v>
+        <v>23.11247378456391</v>
       </c>
       <c r="AJ7">
-        <v>0.5396764877014472</v>
+        <v>0.539675702924542</v>
       </c>
       <c r="AT7" t="s">
         <v>121</v>
@@ -2202,94 +2232,97 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>102.8208864057384</v>
+        <v>102.8205982559851</v>
       </c>
       <c r="D8">
-        <v>102.8280217146328</v>
+        <v>102.8351244661373</v>
       </c>
       <c r="E8">
-        <v>102.8137510968441</v>
+        <v>102.806072045833</v>
       </c>
       <c r="F8" t="s">
         <v>63</v>
       </c>
       <c r="G8">
-        <v>102.758662634727</v>
+        <v>102.7583746593305</v>
+      </c>
+      <c r="H8">
+        <v>0.01958960327781861</v>
+      </c>
+      <c r="I8">
+        <v>0.01435943676881631</v>
       </c>
       <c r="J8">
-        <v>1286.687399168587</v>
+        <v>1286.687722802019</v>
+      </c>
+      <c r="K8">
+        <v>0.01247035261267834</v>
       </c>
       <c r="L8">
-        <v>126.4546076807516</v>
+        <v>126.1765636384594</v>
       </c>
       <c r="M8">
-        <v>1286.687399168587</v>
+        <v>1286.687722802019</v>
       </c>
       <c r="N8">
-        <v>158.1418998726617</v>
+        <v>160.3687132009049</v>
       </c>
       <c r="O8">
-        <v>0.5874211668441253</v>
+        <v>0.5931448825945722</v>
       </c>
       <c r="P8">
-        <v>2.955464845229159</v>
+        <v>2.640592896090385</v>
       </c>
       <c r="Q8">
-        <v>3.527499269129208E-06</v>
+        <v>3.702593787124897E-14</v>
       </c>
       <c r="R8">
-        <v>1.174842333688251</v>
+        <v>1.186289765189144</v>
       </c>
       <c r="S8" t="s">
         <v>115</v>
       </c>
       <c r="T8">
-        <v>1389.446111805815</v>
+        <v>1389.44614746385</v>
       </c>
       <c r="U8">
-        <v>0.0071</v>
+        <v>0.007119250665140266</v>
       </c>
       <c r="V8">
-        <v>211.8332408745676</v>
+        <v>211.8219846285743</v>
       </c>
       <c r="W8">
-        <v>1389.446061803314</v>
+        <v>1389.44609746135</v>
       </c>
       <c r="X8">
-        <v>265.4407204273799</v>
+        <v>265.3448276973129</v>
       </c>
       <c r="Y8">
-        <v>0.5692008961296939</v>
+        <v>0.5692989110669842</v>
+      </c>
+      <c r="Z8">
+        <v>0</v>
       </c>
       <c r="AA8">
-        <v>2.332051626415651</v>
+        <v>2.331539725587954</v>
       </c>
       <c r="AB8">
-        <v>0.1022654607216857</v>
+        <v>0.1008219568759909</v>
       </c>
       <c r="AC8">
-        <v>1.138401792259388</v>
+        <v>1.138597822133968</v>
       </c>
       <c r="AD8" t="s">
         <v>115</v>
       </c>
-      <c r="AE8">
-        <v>1266.481609709411</v>
-      </c>
-      <c r="AF8">
-        <v>10.6160639919987</v>
-      </c>
-      <c r="AG8">
-        <v>0.5446049395078415</v>
-      </c>
       <c r="AH8">
-        <v>1409.462615013279</v>
+        <v>1409.463237821099</v>
       </c>
       <c r="AI8">
-        <v>268.5158073942789</v>
+        <v>268.9485272698817</v>
       </c>
       <c r="AJ8">
-        <v>0.2114869063391098</v>
+        <v>0.2108563242014863</v>
       </c>
       <c r="AT8" t="s">
         <v>63</v>
@@ -2336,91 +2369,88 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>102.7899162208194</v>
+        <v>102.7895680154298</v>
       </c>
       <c r="D9">
-        <v>102.7905723839387</v>
+        <v>102.8038833254448</v>
       </c>
       <c r="E9">
-        <v>102.7892600577002</v>
+        <v>102.7752527054148</v>
       </c>
       <c r="F9" t="s">
         <v>64</v>
       </c>
       <c r="G9">
-        <v>102.7278459989996</v>
+        <v>102.7274980038515</v>
+      </c>
+      <c r="H9">
+        <v>0.01935201509201873</v>
+      </c>
+      <c r="I9">
+        <v>0.01414613921773145</v>
       </c>
       <c r="J9">
-        <v>1286.71813166911</v>
+        <v>1286.718261236902</v>
+      </c>
+      <c r="K9">
+        <v>0.01221204882195297</v>
       </c>
       <c r="L9">
-        <v>118.6414921955403</v>
+        <v>118.3712069097287</v>
       </c>
       <c r="M9">
-        <v>1286.71818167161</v>
+        <v>1286.718261236902</v>
       </c>
       <c r="N9">
-        <v>150.6503697311584</v>
+        <v>152.9912346300638</v>
       </c>
       <c r="O9">
-        <v>0.5964519976875798</v>
+        <v>0.6027299408373412</v>
       </c>
       <c r="P9">
-        <v>2.938489529290651</v>
+        <v>2.535498106193613</v>
       </c>
       <c r="Q9">
-        <v>4.173111856076162E-10</v>
+        <v>1.589177123229035E-10</v>
       </c>
       <c r="R9">
-        <v>1.19290399537516</v>
+        <v>1.205459881674682</v>
       </c>
       <c r="S9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="T9">
-        <v>1389.446027670609</v>
+        <v>1389.445759240753</v>
+      </c>
+      <c r="U9">
+        <v>0.00713996627006576</v>
       </c>
       <c r="V9">
-        <v>194.318971871589</v>
+        <v>194.7497236108655</v>
       </c>
       <c r="W9">
-        <v>1389.446027670609</v>
+        <v>1389.445759240753</v>
       </c>
       <c r="X9">
-        <v>237.7396916867584</v>
+        <v>240.7648242427668</v>
       </c>
       <c r="Y9">
-        <v>0.5694433866066606</v>
+        <v>0.5678424365943296</v>
+      </c>
+      <c r="Z9">
+        <v>0</v>
       </c>
       <c r="AA9">
-        <v>1.948396685359428</v>
+        <v>2.139305002554165</v>
       </c>
       <c r="AB9">
-        <v>0.02825631022199204</v>
+        <v>0.06464257500490034</v>
       </c>
       <c r="AC9">
-        <v>1.138886773213321</v>
+        <v>1.135684873188659</v>
       </c>
       <c r="AD9" t="s">
         <v>115</v>
-      </c>
-      <c r="AE9">
-        <v>1266.562765140663</v>
-      </c>
-      <c r="AF9">
-        <v>47.91626601438467</v>
-      </c>
-      <c r="AG9">
-        <v>0.02986083828304443</v>
-      </c>
-      <c r="AH9">
-        <v>1410.625098543999</v>
-      </c>
-      <c r="AI9">
-        <v>17.47312431683904</v>
-      </c>
-      <c r="AJ9">
-        <v>0.4267433569605878</v>
       </c>
       <c r="AT9" t="s">
         <v>122</v>
@@ -2467,100 +2497,106 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <v>102.8703564170612</v>
+        <v>102.8704180776073</v>
       </c>
       <c r="D10">
-        <v>102.8706523159763</v>
+        <v>102.875047018658</v>
       </c>
       <c r="E10">
-        <v>102.8700605181462</v>
+        <v>102.8657891365566</v>
       </c>
       <c r="F10" t="s">
         <v>65</v>
       </c>
       <c r="G10">
-        <v>102.8075406705368</v>
+        <v>102.8076022934297</v>
+      </c>
+      <c r="H10">
+        <v>0.005068206118767612</v>
+      </c>
+      <c r="I10">
+        <v>0.004113980912890119</v>
       </c>
       <c r="J10">
-        <v>1286.514204893072</v>
+        <v>1286.514192591369</v>
+      </c>
+      <c r="K10">
+        <v>0.003962648179509084</v>
       </c>
       <c r="L10">
-        <v>2008.914260598205</v>
+        <v>2007.852087082756</v>
       </c>
       <c r="M10">
-        <v>1286.514254895572</v>
+        <v>1286.514192591369</v>
       </c>
       <c r="N10">
-        <v>3122.915991113221</v>
+        <v>3102.681441087719</v>
       </c>
       <c r="O10">
-        <v>0.6526552905147924</v>
+        <v>0.652748381001947</v>
       </c>
       <c r="P10">
-        <v>4.204919401373114</v>
+        <v>6.818059220393454</v>
       </c>
       <c r="Q10">
-        <v>0.3296172528337404</v>
+        <v>0.315772567092841</v>
       </c>
       <c r="R10">
-        <v>1.305310581029585</v>
+        <v>1.305496762003894</v>
       </c>
       <c r="S10" t="s">
         <v>115</v>
       </c>
       <c r="T10">
-        <v>1389.321845568609</v>
+        <v>1389.321844887298</v>
+      </c>
+      <c r="U10">
+        <v>0.001105557939258528</v>
       </c>
       <c r="V10">
-        <v>3159.984454362522</v>
+        <v>3159.980343526181</v>
       </c>
       <c r="W10">
-        <v>1389.321795566109</v>
+        <v>1389.321794884798</v>
       </c>
       <c r="X10">
-        <v>4531.58641780378</v>
+        <v>4531.566328952908</v>
       </c>
       <c r="Y10">
-        <v>0.6011756771285541</v>
+        <v>0.6011771161872066</v>
+      </c>
+      <c r="Z10">
+        <v>0</v>
       </c>
       <c r="AA10">
-        <v>4.632487688301636</v>
+        <v>4.636653215110532</v>
       </c>
       <c r="AB10">
-        <v>0.3336844422104223</v>
+        <v>0.3336693903136327</v>
       </c>
       <c r="AC10">
-        <v>1.202351354257108</v>
+        <v>1.202354232374413</v>
       </c>
       <c r="AD10" t="s">
         <v>115</v>
       </c>
-      <c r="AE10">
-        <v>1266.227159805614</v>
-      </c>
-      <c r="AF10">
-        <v>333.6949377337923</v>
-      </c>
-      <c r="AG10">
-        <v>0.7485084566007645</v>
-      </c>
       <c r="AH10">
-        <v>1410.567798852632</v>
+        <v>1410.567798510923</v>
       </c>
       <c r="AI10">
-        <v>476.5994927890397</v>
+        <v>476.5950534041069</v>
       </c>
       <c r="AJ10">
-        <v>0.6422314048185552</v>
+        <v>0.6422349779779991</v>
       </c>
       <c r="AK10">
-        <v>1370.780209677061</v>
+        <v>1370.778733804574</v>
       </c>
       <c r="AL10">
-        <v>68.78535831796582</v>
+        <v>69.83692556896673</v>
       </c>
       <c r="AM10">
-        <v>0.3002648916955102</v>
+        <v>0.3002650831404381</v>
       </c>
       <c r="AT10" t="s">
         <v>123</v>
@@ -2607,112 +2643,115 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <v>102.8668999951187</v>
+        <v>102.8668993206324</v>
       </c>
       <c r="D11">
-        <v>102.8698506981532</v>
+        <v>102.8696070962539</v>
       </c>
       <c r="E11">
-        <v>102.8639492920842</v>
+        <v>102.864191545011</v>
       </c>
       <c r="F11" t="s">
         <v>66</v>
       </c>
       <c r="G11">
-        <v>102.8040676989845</v>
+        <v>102.8040670249084</v>
       </c>
       <c r="H11">
-        <v>0.00379</v>
+        <v>0.002368004918212237</v>
       </c>
       <c r="I11">
-        <v>0.00293429719012918</v>
+        <v>0.001686599101943534</v>
       </c>
       <c r="J11">
-        <v>1286.536041903987</v>
+        <v>1286.536042755235</v>
       </c>
       <c r="K11">
-        <v>0.00274</v>
+        <v>0.001326993515361511</v>
       </c>
       <c r="L11">
-        <v>1867.37187256253</v>
+        <v>1867.371949008568</v>
       </c>
       <c r="M11">
-        <v>1286.536091906487</v>
+        <v>1286.536092757735</v>
       </c>
       <c r="N11">
-        <v>2830.026805143377</v>
+        <v>2830.027034680194</v>
       </c>
       <c r="O11">
-        <v>0.6441902574101334</v>
+        <v>0.6441902123600918</v>
       </c>
       <c r="P11">
-        <v>4.130827135001509</v>
+        <v>4.130839989977289</v>
       </c>
       <c r="Q11">
-        <v>0.2951320235928219</v>
+        <v>0.2951323338430515</v>
       </c>
       <c r="R11">
-        <v>1.288380514820267</v>
+        <v>1.288380424720184</v>
       </c>
       <c r="S11" t="s">
         <v>115</v>
       </c>
       <c r="T11">
-        <v>1389.340209607972</v>
+        <v>1389.340209785143</v>
       </c>
       <c r="U11">
-        <v>0.00105</v>
+        <v>0.001041011402850726</v>
       </c>
       <c r="V11">
-        <v>2912.801363331351</v>
+        <v>2912.801050411318</v>
       </c>
       <c r="W11">
-        <v>1389.340159605472</v>
+        <v>1389.340159782643</v>
       </c>
       <c r="X11">
-        <v>4097.729640104473</v>
+        <v>4097.72808019319</v>
       </c>
       <c r="Y11">
-        <v>0.5956978871889227</v>
+        <v>0.5956980035780688</v>
+      </c>
+      <c r="Z11">
+        <v>0</v>
       </c>
       <c r="AA11">
-        <v>3.677807083267532</v>
+        <v>3.678148669062228</v>
       </c>
       <c r="AB11">
-        <v>0.3057320108676663</v>
+        <v>0.3057307222570549</v>
       </c>
       <c r="AC11">
-        <v>1.191395774377845</v>
+        <v>1.191396007156138</v>
       </c>
       <c r="AD11" t="s">
         <v>115</v>
       </c>
       <c r="AE11">
-        <v>1266.272922893443</v>
+        <v>1266.27292315582</v>
       </c>
       <c r="AF11">
-        <v>313.8405554472529</v>
+        <v>313.8408284805691</v>
       </c>
       <c r="AG11">
-        <v>0.6966487610176202</v>
+        <v>0.6966463909225962</v>
       </c>
       <c r="AH11">
-        <v>1410.586485956184</v>
+        <v>1410.586485958832</v>
       </c>
       <c r="AI11">
-        <v>420.0147821785297</v>
+        <v>420.01447605932</v>
       </c>
       <c r="AJ11">
-        <v>0.6301561964836089</v>
+        <v>0.6301564369739063</v>
       </c>
       <c r="AK11">
-        <v>1370.800342653851</v>
+        <v>1370.80013899863</v>
       </c>
       <c r="AL11">
-        <v>57.24326914478986</v>
+        <v>57.32932404372721</v>
       </c>
       <c r="AM11">
-        <v>0.297539635039088</v>
+        <v>0.297539117208123</v>
       </c>
       <c r="AT11" t="s">
         <v>124</v>
@@ -2759,103 +2798,106 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <v>102.8400577608532</v>
+        <v>102.8400565617631</v>
       </c>
       <c r="D12">
-        <v>102.8418639835001</v>
+        <v>102.8428826717284</v>
       </c>
       <c r="E12">
-        <v>102.8382515382062</v>
+        <v>102.8372304517979</v>
       </c>
       <c r="F12" t="s">
         <v>67</v>
       </c>
       <c r="G12">
-        <v>102.7772240230677</v>
+        <v>102.7772228247079</v>
+      </c>
+      <c r="H12">
+        <v>0.001870245329387664</v>
+      </c>
+      <c r="I12">
+        <v>0.001870245329387664</v>
       </c>
       <c r="J12">
-        <v>1286.565613961279</v>
+        <v>1286.565614277904</v>
       </c>
       <c r="K12">
-        <v>0.00178</v>
+        <v>0.001870245329387664</v>
       </c>
       <c r="L12">
-        <v>1583.912019479877</v>
+        <v>1583.912335892372</v>
       </c>
       <c r="M12">
-        <v>1286.565663963779</v>
+        <v>1286.565664280404</v>
       </c>
       <c r="N12">
-        <v>2353.181434212452</v>
+        <v>2353.181715891018</v>
       </c>
       <c r="O12">
-        <v>0.6309336198132111</v>
+        <v>0.6309333567748598</v>
       </c>
       <c r="P12">
-        <v>3.409027440891033</v>
+        <v>3.409033950406637</v>
       </c>
       <c r="Q12">
-        <v>0.2976724365878834</v>
+        <v>0.2976733861160941</v>
       </c>
       <c r="R12">
-        <v>1.261867239626422</v>
+        <v>1.26186671354972</v>
       </c>
       <c r="S12" t="s">
         <v>115</v>
       </c>
       <c r="T12">
-        <v>1389.342937989346</v>
+        <v>1389.342937107612</v>
+      </c>
+      <c r="U12">
+        <v>0</v>
       </c>
       <c r="V12">
-        <v>2496.634724744991</v>
+        <v>2496.839558386462</v>
       </c>
       <c r="W12">
-        <v>1389.342887986846</v>
+        <v>1389.342887105112</v>
       </c>
       <c r="X12">
-        <v>3480.050696420718</v>
+        <v>3480.944999477682</v>
       </c>
       <c r="Y12">
-        <v>0.586742003609601</v>
+        <v>0.5866546197763858</v>
+      </c>
+      <c r="Z12">
+        <v>0</v>
       </c>
       <c r="AA12">
-        <v>4.155197464541771</v>
+        <v>4.503521419654371</v>
       </c>
       <c r="AB12">
-        <v>0.3223060693312403</v>
+        <v>0.3231930855962449</v>
       </c>
       <c r="AC12">
-        <v>1.173484007219202</v>
+        <v>1.173309239552772</v>
       </c>
       <c r="AD12" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="AE12">
-        <v>1266.288326968617</v>
+        <v>1266.288328106595</v>
       </c>
       <c r="AF12">
-        <v>260.4092680589347</v>
+        <v>260.410258142661</v>
       </c>
       <c r="AG12">
-        <v>0.6834611580882213</v>
+        <v>0.683452164344494</v>
       </c>
       <c r="AH12">
-        <v>1410.617128229772</v>
+        <v>1410.617124977803</v>
       </c>
       <c r="AI12">
-        <v>364.0307205016263</v>
+        <v>364.201738355314</v>
       </c>
       <c r="AJ12">
-        <v>0.6193241887705594</v>
-      </c>
-      <c r="AK12">
-        <v>1370.813596456425</v>
-      </c>
-      <c r="AL12">
-        <v>44.37567273108929</v>
-      </c>
-      <c r="AM12">
-        <v>0.2930389992530438</v>
+        <v>0.6191432416580879</v>
       </c>
       <c r="AT12" t="s">
         <v>67</v>
@@ -2902,103 +2944,115 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <v>102.8441957158469</v>
+        <v>102.8442060419627</v>
       </c>
       <c r="D13">
-        <v>102.8456023194993</v>
+        <v>102.8468170033194</v>
       </c>
       <c r="E13">
-        <v>102.8427891121946</v>
+        <v>102.8415950806061</v>
       </c>
       <c r="F13" t="s">
         <v>68</v>
       </c>
       <c r="G13">
-        <v>102.7813471705254</v>
+        <v>102.781357490328</v>
+      </c>
+      <c r="H13">
+        <v>0.002091182321466171</v>
+      </c>
+      <c r="I13">
+        <v>0.001525210211436101</v>
       </c>
       <c r="J13">
-        <v>1286.58434964045</v>
+        <v>1286.584350370463</v>
       </c>
       <c r="K13">
-        <v>0.00137</v>
+        <v>0.001309924698392076</v>
       </c>
       <c r="L13">
-        <v>1310.046538675736</v>
+        <v>1310.046114728106</v>
       </c>
       <c r="M13">
-        <v>1286.58439964295</v>
+        <v>1286.584400372963</v>
       </c>
       <c r="N13">
-        <v>1945.264508270439</v>
+        <v>1945.263192442347</v>
       </c>
       <c r="O13">
-        <v>0.638156057461966</v>
+        <v>0.6381565052003531</v>
       </c>
       <c r="P13">
-        <v>2.870289284049282</v>
+        <v>2.870287111102698</v>
       </c>
       <c r="Q13">
-        <v>0.2639659338727581</v>
+        <v>0.2639629370421149</v>
       </c>
       <c r="R13">
-        <v>1.276312114923932</v>
+        <v>1.276313010400706</v>
       </c>
       <c r="S13" t="s">
         <v>115</v>
       </c>
       <c r="T13">
-        <v>1389.365796815976</v>
+        <v>1389.365807865791</v>
+      </c>
+      <c r="U13">
+        <v>0.0007812576230740952</v>
       </c>
       <c r="V13">
-        <v>2068.595834111156</v>
+        <v>2068.608488293247</v>
       </c>
       <c r="W13">
-        <v>1389.365746813475</v>
+        <v>1389.365757863291</v>
       </c>
       <c r="X13">
-        <v>2858.976195189386</v>
+        <v>2859.036192373171</v>
       </c>
       <c r="Y13">
-        <v>0.5896167585703433</v>
+        <v>0.5896104211723812</v>
+      </c>
+      <c r="Z13">
+        <v>0</v>
       </c>
       <c r="AA13">
-        <v>2.925351511344183</v>
+        <v>2.935798820233474</v>
       </c>
       <c r="AB13">
-        <v>0.2847920672120289</v>
+        <v>0.2848629599359259</v>
       </c>
       <c r="AC13">
-        <v>1.179233517140687</v>
+        <v>1.179220842344762</v>
       </c>
       <c r="AD13" t="s">
         <v>115</v>
       </c>
       <c r="AE13">
-        <v>1266.315190607358</v>
+        <v>1266.315190811144</v>
       </c>
       <c r="AF13">
-        <v>191.0197512725757</v>
+        <v>191.018783493495</v>
       </c>
       <c r="AG13">
-        <v>0.7148731489816416</v>
+        <v>0.7148753449040686</v>
       </c>
       <c r="AH13">
-        <v>1410.61349017381</v>
+        <v>1410.613489928494</v>
       </c>
       <c r="AI13">
-        <v>292.4890936308656</v>
+        <v>292.4977288959921</v>
       </c>
       <c r="AJ13">
-        <v>0.6049404630671454</v>
+        <v>0.604928037291371</v>
       </c>
       <c r="AK13">
-        <v>1371.186065479649</v>
+        <v>1370.819105890403</v>
       </c>
       <c r="AL13">
-        <v>42.38028606710211</v>
+        <v>40.60721066799029</v>
       </c>
       <c r="AM13">
-        <v>0.2944792148548661</v>
+        <v>0.2944795075430687</v>
       </c>
       <c r="AT13" t="s">
         <v>68</v>
@@ -3045,103 +3099,106 @@
         <v>0</v>
       </c>
       <c r="C14">
-        <v>102.834180349311</v>
+        <v>102.8341902662059</v>
       </c>
       <c r="D14">
-        <v>102.8365908488731</v>
+        <v>102.8375546461059</v>
       </c>
       <c r="E14">
-        <v>102.8317698497489</v>
+        <v>102.8308258863059</v>
       </c>
       <c r="F14" t="s">
         <v>69</v>
       </c>
       <c r="G14">
-        <v>102.7713274842895</v>
+        <v>102.7713373951196</v>
+      </c>
+      <c r="H14">
+        <v>0.003315378235690894</v>
+      </c>
+      <c r="I14">
+        <v>0.002611550130060168</v>
       </c>
       <c r="J14">
-        <v>1286.598044746033</v>
+        <v>1286.598046284791</v>
       </c>
       <c r="K14">
-        <v>0.00239</v>
+        <v>0.002471423613541325</v>
       </c>
       <c r="L14">
-        <v>1088.256533143961</v>
+        <v>1088.256975254012</v>
       </c>
       <c r="M14">
-        <v>1286.598094748533</v>
+        <v>1286.598096287291</v>
       </c>
       <c r="N14">
-        <v>1595.734031515814</v>
+        <v>1595.734872302461</v>
       </c>
       <c r="O14">
-        <v>0.6327017632761961</v>
+        <v>0.6327012611713856</v>
       </c>
       <c r="P14">
-        <v>2.771016323568558</v>
+        <v>2.771013160145491</v>
       </c>
       <c r="Q14">
-        <v>0.252600928266034</v>
+        <v>0.2526035292366982</v>
       </c>
       <c r="R14">
-        <v>1.265403526552392</v>
+        <v>1.265402522342771</v>
       </c>
       <c r="S14" t="s">
         <v>115</v>
       </c>
       <c r="T14">
-        <v>1389.369472235323</v>
+        <v>1389.369483684911</v>
+      </c>
+      <c r="U14">
+        <v>0.0008439546221495684</v>
       </c>
       <c r="V14">
-        <v>1734.069664924798</v>
+        <v>1734.081130528175</v>
       </c>
       <c r="W14">
-        <v>1389.369422232823</v>
+        <v>1389.369433682411</v>
       </c>
       <c r="X14">
-        <v>2394.394673795377</v>
+        <v>2394.450116341764</v>
       </c>
       <c r="Y14">
-        <v>0.5951991800405249</v>
+        <v>0.595192182131449</v>
+      </c>
+      <c r="Z14">
+        <v>0</v>
       </c>
       <c r="AA14">
-        <v>3.081093746093225</v>
+        <v>3.06941149636121</v>
       </c>
       <c r="AB14">
-        <v>0.2554292567826676</v>
+        <v>0.255508679558714</v>
       </c>
       <c r="AC14">
-        <v>1.19039836008105</v>
+        <v>1.190384364262898</v>
       </c>
       <c r="AD14" t="s">
         <v>115</v>
       </c>
       <c r="AE14">
-        <v>1266.305772132352</v>
+        <v>1266.305772533881</v>
       </c>
       <c r="AF14">
-        <v>159.1159683540576</v>
+        <v>159.1151343164653</v>
       </c>
       <c r="AG14">
-        <v>0.6917689508095292</v>
+        <v>0.6917707244572139</v>
       </c>
       <c r="AH14">
-        <v>1410.596943087426</v>
+        <v>1410.596942867364</v>
       </c>
       <c r="AI14">
-        <v>239.9916109260897</v>
+        <v>240.0006505571608</v>
       </c>
       <c r="AJ14">
-        <v>0.6030968802307942</v>
-      </c>
-      <c r="AK14">
-        <v>1372.683385870967</v>
-      </c>
-      <c r="AL14">
-        <v>2.090000749131144</v>
-      </c>
-      <c r="AM14">
-        <v>0.2973297400900483</v>
+        <v>0.6030833360381023</v>
       </c>
       <c r="AT14" t="s">
         <v>69</v>
@@ -3188,103 +3245,115 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <v>102.8318300106004</v>
+        <v>102.8318426608749</v>
       </c>
       <c r="D15">
-        <v>102.8332963382598</v>
+        <v>102.8347100453125</v>
       </c>
       <c r="E15">
-        <v>102.8303636829411</v>
+        <v>102.8289752764372</v>
       </c>
       <c r="F15" t="s">
         <v>70</v>
       </c>
       <c r="G15">
-        <v>102.7689719120613</v>
+        <v>102.7689845545988</v>
+      </c>
+      <c r="H15">
+        <v>0.00271610152078743</v>
+      </c>
+      <c r="I15">
+        <v>0.001929572920964801</v>
       </c>
       <c r="J15">
-        <v>1286.609900147807</v>
+        <v>1286.609899759972</v>
       </c>
       <c r="K15">
-        <v>0.00143</v>
+        <v>0.001489671278757565</v>
       </c>
       <c r="L15">
-        <v>1029.254437868277</v>
+        <v>1029.25451807488</v>
       </c>
       <c r="M15">
-        <v>1286.609950150307</v>
+        <v>1286.609949762473</v>
       </c>
       <c r="N15">
-        <v>1500.31350357264</v>
+        <v>1500.313540463477</v>
       </c>
       <c r="O15">
-        <v>0.623761509536745</v>
+        <v>0.6237614136447998</v>
       </c>
       <c r="P15">
-        <v>2.52279136986443</v>
+        <v>2.522792122775846</v>
       </c>
       <c r="Q15">
-        <v>0.2762462276161498</v>
+        <v>0.2762465110654987</v>
       </c>
       <c r="R15">
-        <v>1.24752301907349</v>
+        <v>1.2475228272896</v>
       </c>
       <c r="S15" t="s">
         <v>115</v>
       </c>
       <c r="T15">
-        <v>1389.378972064869</v>
+        <v>1389.378984319571</v>
+      </c>
+      <c r="U15">
+        <v>0.001226430242029865</v>
       </c>
       <c r="V15">
-        <v>1592.142017277545</v>
+        <v>1592.15197831021</v>
       </c>
       <c r="W15">
-        <v>1389.378922062369</v>
+        <v>1389.378934317071</v>
       </c>
       <c r="X15">
-        <v>2181.879939253626</v>
+        <v>2181.928217022015</v>
       </c>
       <c r="Y15">
-        <v>0.5904113503049053</v>
+        <v>0.5904048635006208</v>
+      </c>
+      <c r="Z15">
+        <v>0</v>
       </c>
       <c r="AA15">
-        <v>2.508229900713894</v>
+        <v>2.527353769313759</v>
       </c>
       <c r="AB15">
-        <v>0.2568950697193793</v>
+        <v>0.2569700972851313</v>
       </c>
       <c r="AC15">
-        <v>1.180822700609811</v>
+        <v>1.180809727001242</v>
       </c>
       <c r="AD15" t="s">
         <v>115</v>
       </c>
       <c r="AE15">
-        <v>1266.332772569196</v>
+        <v>1266.332772301274</v>
       </c>
       <c r="AF15">
-        <v>157.9681117429605</v>
+        <v>157.9680704945629</v>
       </c>
       <c r="AG15">
-        <v>0.6127681757915584</v>
+        <v>0.6127685353989395</v>
       </c>
       <c r="AH15">
-        <v>1410.623124127106</v>
+        <v>1410.623123732466</v>
       </c>
       <c r="AI15">
-        <v>200.708113523828</v>
+        <v>200.714819923112</v>
       </c>
       <c r="AJ15">
-        <v>0.6342349870022564</v>
+        <v>0.6342253480112078</v>
       </c>
       <c r="AK15">
-        <v>1371.206208516615</v>
+        <v>1370.808413720606</v>
       </c>
       <c r="AL15">
-        <v>31.34689526877638</v>
+        <v>29.83449719172587</v>
       </c>
       <c r="AM15">
-        <v>0.2949199428794577</v>
+        <v>0.2949201538677559</v>
       </c>
       <c r="AT15" t="s">
         <v>70</v>
@@ -3331,103 +3400,115 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <v>102.8231150287799</v>
+        <v>102.8231149704386</v>
       </c>
       <c r="D16">
-        <v>102.8249779726709</v>
+        <v>102.8260086566734</v>
       </c>
       <c r="E16">
-        <v>102.8212520848889</v>
+        <v>102.8202212842037</v>
       </c>
       <c r="F16" t="s">
         <v>71</v>
       </c>
       <c r="G16">
-        <v>102.7602610841025</v>
+        <v>102.7602610257916</v>
+      </c>
+      <c r="H16">
+        <v>0.002649801532476578</v>
+      </c>
+      <c r="I16">
+        <v>0.001967270063588711</v>
       </c>
       <c r="J16">
-        <v>1286.618255768769</v>
+        <v>1286.6182563198</v>
       </c>
       <c r="K16">
-        <v>0.00183</v>
+        <v>0.001748827306062537</v>
       </c>
       <c r="L16">
-        <v>869.1157430401952</v>
+        <v>869.1143501581955</v>
       </c>
       <c r="M16">
-        <v>1286.618305771269</v>
+        <v>1286.6183063223</v>
       </c>
       <c r="N16">
-        <v>1250.244634384739</v>
+        <v>1250.242583729209</v>
       </c>
       <c r="O16">
-        <v>0.6332213252611365</v>
+        <v>0.6332233928610588</v>
       </c>
       <c r="P16">
-        <v>2.456918365709782</v>
+        <v>2.456909353240618</v>
       </c>
       <c r="Q16">
-        <v>0.1951249024560196</v>
+        <v>0.1951153009217559</v>
       </c>
       <c r="R16">
-        <v>1.266442650522273</v>
+        <v>1.266446785722118</v>
       </c>
       <c r="S16" t="s">
         <v>115</v>
       </c>
       <c r="T16">
-        <v>1389.378616857871</v>
+        <v>1389.378617350591</v>
+      </c>
+      <c r="U16">
+        <v>0.0009009742264140405</v>
       </c>
       <c r="V16">
-        <v>1391.178505754601</v>
+        <v>1391.176408884319</v>
       </c>
       <c r="W16">
-        <v>1389.378566855371</v>
+        <v>1389.378567348091</v>
       </c>
       <c r="X16">
-        <v>1895.855049607739</v>
+        <v>1895.846206429386</v>
       </c>
       <c r="Y16">
-        <v>0.5834382813884054</v>
+        <v>0.5834398540904167</v>
+      </c>
+      <c r="Z16">
+        <v>0</v>
       </c>
       <c r="AA16">
-        <v>2.275619967584088</v>
+        <v>2.277279250434276</v>
       </c>
       <c r="AB16">
-        <v>0.2747677007865592</v>
+        <v>0.2747514015585826</v>
       </c>
       <c r="AC16">
-        <v>1.166876562776811</v>
+        <v>1.166879708180833</v>
       </c>
       <c r="AD16" t="s">
         <v>115</v>
       </c>
       <c r="AE16">
-        <v>1266.318666461496</v>
+        <v>1266.318666400955</v>
       </c>
       <c r="AF16">
-        <v>122.4809359100691</v>
+        <v>122.4809914561068</v>
       </c>
       <c r="AG16">
-        <v>0.6949018867091679</v>
+        <v>0.6949020541179575</v>
       </c>
       <c r="AH16">
-        <v>1410.617805704099</v>
+        <v>1410.617805912265</v>
       </c>
       <c r="AI16">
-        <v>185.1406816347607</v>
+        <v>185.1390250480642</v>
       </c>
       <c r="AJ16">
-        <v>0.6086692417715888</v>
+        <v>0.6086722333255329</v>
       </c>
       <c r="AK16">
-        <v>1371.199690057767</v>
+        <v>1371.201354087113</v>
       </c>
       <c r="AL16">
-        <v>28.88581738337454</v>
+        <v>29.32751195876292</v>
       </c>
       <c r="AM16">
-        <v>0.2914073765873408</v>
+        <v>0.29140765886788</v>
       </c>
       <c r="AT16" t="s">
         <v>71</v>
@@ -3474,112 +3555,106 @@
         <v>0</v>
       </c>
       <c r="C17">
-        <v>102.8147162723139</v>
+        <v>102.8147148211203</v>
       </c>
       <c r="D17">
-        <v>102.8159879141655</v>
+        <v>102.8170755543238</v>
       </c>
       <c r="E17">
-        <v>102.8134446304624</v>
+        <v>102.8123540879168</v>
       </c>
       <c r="F17" t="s">
         <v>72</v>
       </c>
       <c r="G17">
-        <v>102.7518731468704</v>
+        <v>102.7518716965576</v>
       </c>
       <c r="H17">
-        <v>0.001675</v>
+        <v>0.001034206157417467</v>
       </c>
       <c r="I17">
-        <v>0.001218533955210112</v>
+        <v>0.001034206157417467</v>
       </c>
       <c r="J17">
-        <v>1286.640248463998</v>
+        <v>1286.640300372685</v>
       </c>
       <c r="K17">
-        <v>0.000635</v>
+        <v>0</v>
       </c>
       <c r="L17">
-        <v>750.9688354372702</v>
+        <v>751.237991028744</v>
       </c>
       <c r="M17">
-        <v>1286.640298466498</v>
+        <v>1286.640300372685</v>
       </c>
       <c r="N17">
-        <v>1062.86707453755</v>
+        <v>1064.014664873351</v>
       </c>
       <c r="O17">
-        <v>0.6157652272220931</v>
+        <v>0.6153214929720126</v>
       </c>
       <c r="P17">
-        <v>2.422797154313316</v>
+        <v>3.207466719717423</v>
       </c>
       <c r="Q17">
-        <v>0.2288955292752605</v>
+        <v>0.2331553386480496</v>
       </c>
       <c r="R17">
-        <v>1.231530454444186</v>
+        <v>1.230642985944025</v>
       </c>
       <c r="S17" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="T17">
-        <v>1389.392221615869</v>
+        <v>1389.392222071742</v>
       </c>
       <c r="U17">
-        <v>0.00104</v>
+        <v>0.001034206157417467</v>
       </c>
       <c r="V17">
-        <v>1184.449414069262</v>
+        <v>1184.449291077927</v>
       </c>
       <c r="W17">
-        <v>1389.392171613369</v>
+        <v>1389.392172069242</v>
       </c>
       <c r="X17">
-        <v>1601.610566246641</v>
+        <v>1601.610118603454</v>
       </c>
       <c r="Y17">
-        <v>0.5876006684207854</v>
+        <v>0.5876007761986123</v>
+      </c>
+      <c r="Z17">
+        <v>0</v>
       </c>
       <c r="AA17">
-        <v>2.110571388063803</v>
+        <v>2.11060679583484</v>
       </c>
       <c r="AB17">
-        <v>0.2323201570047335</v>
+        <v>0.2323191326516478</v>
       </c>
       <c r="AC17">
-        <v>1.175201336841571</v>
+        <v>1.175201552397225</v>
       </c>
       <c r="AD17" t="s">
         <v>115</v>
       </c>
-      <c r="AE17">
-        <v>1266.296042570815</v>
-      </c>
-      <c r="AF17">
-        <v>95.39795068665839</v>
-      </c>
-      <c r="AG17">
-        <v>0.6558146636274728</v>
-      </c>
       <c r="AH17">
-        <v>1410.639581620845</v>
+        <v>1410.639581782064</v>
       </c>
       <c r="AI17">
-        <v>152.0124241854188</v>
+        <v>152.012400241478</v>
       </c>
       <c r="AJ17">
-        <v>0.6132423788131017</v>
+        <v>0.6132424390069341</v>
       </c>
       <c r="AK17">
-        <v>1370.833553059655</v>
+        <v>1370.833453104975</v>
       </c>
       <c r="AL17">
-        <v>22.79458870662697</v>
+        <v>22.80440667693624</v>
       </c>
       <c r="AM17">
-        <v>0.2935149611925038</v>
+        <v>0.2935148530137768</v>
       </c>
       <c r="AT17" t="s">
         <v>72</v>
@@ -3626,94 +3701,97 @@
         <v>0</v>
       </c>
       <c r="C18">
-        <v>102.8167516416584</v>
+        <v>102.8167569521262</v>
       </c>
       <c r="D18">
-        <v>102.8181325678289</v>
+        <v>102.819280175819</v>
       </c>
       <c r="E18">
-        <v>102.8153707154879</v>
+        <v>102.8142337284334</v>
       </c>
       <c r="F18" t="s">
         <v>73</v>
       </c>
       <c r="G18">
-        <v>102.7539184948616</v>
+        <v>102.753923802077</v>
+      </c>
+      <c r="H18">
+        <v>0.001362976805101453</v>
+      </c>
+      <c r="I18">
+        <v>0.001362976805101453</v>
       </c>
       <c r="J18">
-        <v>1286.643880416629</v>
+        <v>1286.643925304705</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
       </c>
       <c r="L18">
-        <v>644.8889172444638</v>
+        <v>644.8280989129333</v>
       </c>
       <c r="M18">
-        <v>1286.643930419129</v>
+        <v>1286.643925304705</v>
       </c>
       <c r="N18">
-        <v>903.9230833677728</v>
+        <v>902.6063240202728</v>
       </c>
       <c r="O18">
-        <v>0.6164965214377255</v>
+        <v>0.6164199160431029</v>
       </c>
       <c r="P18">
-        <v>2.079447600751909</v>
+        <v>2.748847949519055</v>
       </c>
       <c r="Q18">
-        <v>0.1974300096017826</v>
+        <v>0.1948225714790455</v>
       </c>
       <c r="R18">
-        <v>1.232993042875451</v>
+        <v>1.232839832086206</v>
       </c>
       <c r="S18" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="T18">
-        <v>1389.397898916491</v>
+        <v>1389.397899109282</v>
       </c>
       <c r="U18">
-        <v>0.00133</v>
+        <v>0.001362976805101453</v>
       </c>
       <c r="V18">
-        <v>1011.988248429066</v>
+        <v>1011.988106114069</v>
       </c>
       <c r="W18">
-        <v>1389.397848913991</v>
+        <v>1389.397849106782</v>
       </c>
       <c r="X18">
-        <v>1351.285016208558</v>
+        <v>1351.284811499432</v>
       </c>
       <c r="Y18">
-        <v>0.5865573610916996</v>
+        <v>0.5865575201867601</v>
+      </c>
+      <c r="Z18">
+        <v>0</v>
       </c>
       <c r="AA18">
-        <v>2.098068931806045</v>
+        <v>2.098066966675925</v>
       </c>
       <c r="AB18">
-        <v>0.2011078611746406</v>
+        <v>0.2011070428846714</v>
       </c>
       <c r="AC18">
-        <v>1.173114722183399</v>
+        <v>1.17311504037352</v>
       </c>
       <c r="AD18" t="s">
         <v>115</v>
       </c>
-      <c r="AE18">
-        <v>1266.358352835361</v>
-      </c>
-      <c r="AF18">
-        <v>76.75604393487586</v>
-      </c>
-      <c r="AG18">
-        <v>0.6941464113149803</v>
-      </c>
       <c r="AH18">
-        <v>1410.61385297202</v>
+        <v>1410.613852864538</v>
       </c>
       <c r="AI18">
-        <v>129.442653492253</v>
+        <v>129.442679800638</v>
       </c>
       <c r="AJ18">
-        <v>0.6054114123296602</v>
+        <v>0.6054112918911643</v>
       </c>
       <c r="AT18" t="s">
         <v>73</v>
@@ -3760,100 +3838,106 @@
         <v>0</v>
       </c>
       <c r="C19">
-        <v>102.8216421957285</v>
+        <v>102.821667774588</v>
       </c>
       <c r="D19">
-        <v>102.8220149777594</v>
+        <v>102.8259083538401</v>
       </c>
       <c r="E19">
-        <v>102.8212694136975</v>
+        <v>102.8174271953358</v>
       </c>
       <c r="F19" t="s">
         <v>74</v>
       </c>
       <c r="G19">
-        <v>102.7588262154188</v>
+        <v>102.7588517786435</v>
+      </c>
+      <c r="H19">
+        <v>0.004794680859407258</v>
+      </c>
+      <c r="I19">
+        <v>0.003667941745570606</v>
       </c>
       <c r="J19">
-        <v>1286.652539124805</v>
+        <v>1286.652572791544</v>
+      </c>
+      <c r="K19">
+        <v>0.003387116762295085</v>
       </c>
       <c r="L19">
-        <v>516.7400623057168</v>
+        <v>516.557276254901</v>
       </c>
       <c r="M19">
-        <v>1286.652589127305</v>
+        <v>1286.652572791544</v>
       </c>
       <c r="N19">
-        <v>708.9240860289054</v>
+        <v>706.9587189701974</v>
       </c>
       <c r="O19">
-        <v>0.6019897191602857</v>
+        <v>0.6021250735905106</v>
       </c>
       <c r="P19">
-        <v>1.977681976479061</v>
+        <v>2.484142062301762</v>
       </c>
       <c r="Q19">
-        <v>0.2043081818531133</v>
+        <v>0.1980529517441689</v>
       </c>
       <c r="R19">
-        <v>1.203979438320571</v>
+        <v>1.204250147181021</v>
       </c>
       <c r="S19" t="s">
         <v>115</v>
       </c>
       <c r="T19">
-        <v>1389.411465345224</v>
+        <v>1389.411474572688</v>
+      </c>
+      <c r="U19">
+        <v>0.001407564097112173</v>
       </c>
       <c r="V19">
-        <v>792.9448128715991</v>
+        <v>792.8747237344076</v>
       </c>
       <c r="W19">
-        <v>1389.411415342724</v>
+        <v>1389.411424570188</v>
       </c>
       <c r="X19">
-        <v>1051.898793616349</v>
+        <v>1051.576005716134</v>
       </c>
       <c r="Y19">
-        <v>0.5868226947242257</v>
+        <v>0.5869147013583159</v>
+      </c>
+      <c r="Z19">
+        <v>0</v>
       </c>
       <c r="AA19">
-        <v>2.034857871515118</v>
+        <v>1.908237395171035</v>
       </c>
       <c r="AB19">
-        <v>0.1807415312027706</v>
+        <v>0.1796610706278235</v>
       </c>
       <c r="AC19">
-        <v>1.173645389448451</v>
+        <v>1.173829402716632</v>
       </c>
       <c r="AD19" t="s">
         <v>115</v>
       </c>
-      <c r="AE19">
-        <v>1266.37089434768</v>
-      </c>
-      <c r="AF19">
-        <v>59.80124269598025</v>
-      </c>
-      <c r="AG19">
-        <v>0.6480697016290011</v>
-      </c>
       <c r="AH19">
-        <v>1410.642629847099</v>
+        <v>1410.642629173379</v>
       </c>
       <c r="AI19">
-        <v>100.378243717975</v>
+        <v>100.3219180950477</v>
       </c>
       <c r="AJ19">
-        <v>0.5817608708021854</v>
+        <v>0.5819477949179205</v>
       </c>
       <c r="AK19">
-        <v>1369.437022511488</v>
+        <v>1371.212385465681</v>
       </c>
       <c r="AL19">
-        <v>3.380230752839193</v>
+        <v>18.68571662292745</v>
       </c>
       <c r="AM19">
-        <v>0.2931767092253595</v>
+        <v>0.2931766618605695</v>
       </c>
       <c r="AT19" t="s">
         <v>74</v>
@@ -3900,94 +3984,97 @@
         <v>0</v>
       </c>
       <c r="C20">
-        <v>102.8097259908781</v>
+        <v>102.8097325206188</v>
       </c>
       <c r="D20">
-        <v>102.8120476384815</v>
+        <v>102.8128201838124</v>
       </c>
       <c r="E20">
-        <v>102.8074043432746</v>
+        <v>102.8066448574252</v>
       </c>
       <c r="F20" t="s">
         <v>75</v>
       </c>
       <c r="G20">
-        <v>102.7469606169641</v>
+        <v>102.7469671427086</v>
+      </c>
+      <c r="H20">
+        <v>0.002237983949013372</v>
+      </c>
+      <c r="I20">
+        <v>0.002237983949013372</v>
       </c>
       <c r="J20">
-        <v>1286.664017398754</v>
+        <v>1286.664009539184</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
       </c>
       <c r="L20">
-        <v>369.8389927018004</v>
+        <v>370.4422194541194</v>
       </c>
       <c r="M20">
-        <v>1286.664017398754</v>
+        <v>1286.664009539184</v>
       </c>
       <c r="N20">
-        <v>491.8266773563823</v>
+        <v>496.1665866317188</v>
       </c>
       <c r="O20">
-        <v>0.611278174530538</v>
+        <v>0.609913377947215</v>
       </c>
       <c r="P20">
-        <v>1.971002198859888</v>
+        <v>2.175262265911358</v>
       </c>
       <c r="Q20">
-        <v>0.0664141340161612</v>
+        <v>0.09212873242437403</v>
       </c>
       <c r="R20">
-        <v>1.222556349061076</v>
+        <v>1.21982675589443</v>
       </c>
       <c r="S20" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="T20">
-        <v>1389.411028018218</v>
+        <v>1389.411026684393</v>
       </c>
       <c r="U20">
-        <v>0.00228</v>
+        <v>0.002237983949013372</v>
       </c>
       <c r="V20">
-        <v>579.8559416747313</v>
+        <v>579.8561129814287</v>
       </c>
       <c r="W20">
-        <v>1389.410978015718</v>
+        <v>1389.410976681893</v>
       </c>
       <c r="X20">
-        <v>766.0533195650653</v>
+        <v>766.0535950356493</v>
       </c>
       <c r="Y20">
-        <v>0.5812471601064908</v>
+        <v>0.5812468357340371</v>
+      </c>
+      <c r="Z20">
+        <v>0</v>
       </c>
       <c r="AA20">
-        <v>1.925108776966211</v>
+        <v>1.925110247186574</v>
       </c>
       <c r="AB20">
-        <v>0.1965385388217322</v>
+        <v>0.1965403501772163</v>
       </c>
       <c r="AC20">
-        <v>1.162494320212982</v>
+        <v>1.162493671468074</v>
       </c>
       <c r="AD20" t="s">
         <v>115</v>
       </c>
-      <c r="AE20">
-        <v>1266.349327948957</v>
-      </c>
-      <c r="AF20">
-        <v>32.75050151801313</v>
-      </c>
-      <c r="AG20">
-        <v>0.576499779564984</v>
-      </c>
       <c r="AH20">
-        <v>1410.633980810806</v>
+        <v>1410.633982096898</v>
       </c>
       <c r="AI20">
-        <v>74.86176745341729</v>
+        <v>74.86204761641844</v>
       </c>
       <c r="AJ20">
-        <v>0.5819797521974224</v>
+        <v>0.5819760710383698</v>
       </c>
       <c r="AT20" t="s">
         <v>75</v>
@@ -4034,94 +4121,97 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <v>102.7888242426879</v>
+        <v>102.7888154091925</v>
       </c>
       <c r="D21">
-        <v>102.7913743781052</v>
+        <v>102.7920994834932</v>
       </c>
       <c r="E21">
-        <v>102.7862741072705</v>
+        <v>102.7855313348918</v>
       </c>
       <c r="F21" t="s">
         <v>76</v>
       </c>
       <c r="G21">
-        <v>102.7261013957564</v>
+        <v>102.7260925676405</v>
+      </c>
+      <c r="H21">
+        <v>0.002501228481495914</v>
+      </c>
+      <c r="I21">
+        <v>0.002501228481495914</v>
       </c>
       <c r="J21">
-        <v>1286.691022302416</v>
+        <v>1286.69103359793</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
       </c>
       <c r="L21">
-        <v>254.1738183660939</v>
+        <v>254.9590919673388</v>
       </c>
       <c r="M21">
-        <v>1286.691022302416</v>
+        <v>1286.69103359793</v>
       </c>
       <c r="N21">
-        <v>328.4230722390374</v>
+        <v>333.9762239991902</v>
       </c>
       <c r="O21">
-        <v>0.6068868614370199</v>
+        <v>0.6044432659842554</v>
       </c>
       <c r="P21">
-        <v>1.962703469782377</v>
+        <v>2.099901996957981</v>
       </c>
       <c r="Q21">
-        <v>0.0002350275441995731</v>
+        <v>0.04923933915745116</v>
       </c>
       <c r="R21">
-        <v>1.21377372287404</v>
+        <v>1.208886531968511</v>
       </c>
       <c r="S21" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="T21">
-        <v>1389.417173700672</v>
+        <v>1389.41717616807</v>
       </c>
       <c r="U21">
-        <v>0.00251</v>
+        <v>0.002501228481495914</v>
       </c>
       <c r="V21">
-        <v>403.3441591565559</v>
+        <v>403.3441183043637</v>
       </c>
       <c r="W21">
-        <v>1389.417123698172</v>
+        <v>1389.41712616557</v>
       </c>
       <c r="X21">
-        <v>521.1721870804433</v>
+        <v>521.1720523797705</v>
       </c>
       <c r="Y21">
-        <v>0.5799251551644382</v>
+        <v>0.5799252496106378</v>
+      </c>
+      <c r="Z21">
+        <v>0</v>
       </c>
       <c r="AA21">
-        <v>1.695961527078159</v>
+        <v>1.695961219440426</v>
       </c>
       <c r="AB21">
-        <v>0.1380803386491486</v>
+        <v>0.1380793976884254</v>
       </c>
       <c r="AC21">
-        <v>1.159850310328876</v>
+        <v>1.159850499221276</v>
       </c>
       <c r="AD21" t="s">
         <v>115</v>
       </c>
-      <c r="AE21">
-        <v>1266.362019146426</v>
-      </c>
-      <c r="AF21">
-        <v>27.17575084310541</v>
-      </c>
-      <c r="AG21">
-        <v>0.6427437398759817</v>
-      </c>
       <c r="AH21">
-        <v>1410.682841314734</v>
+        <v>1410.682848991785</v>
       </c>
       <c r="AI21">
-        <v>49.43147424978309</v>
+        <v>49.43198796888679</v>
       </c>
       <c r="AJ21">
-        <v>0.5917359852045998</v>
+        <v>0.5917279829662407</v>
       </c>
       <c r="AT21" t="s">
         <v>76</v>
@@ -4168,13 +4258,13 @@
         <v>0</v>
       </c>
       <c r="C22">
-        <v>105.0099627176329</v>
+        <v>105.0099627176341</v>
       </c>
       <c r="D22">
-        <v>105.0114169763005</v>
+        <v>105.0125389023183</v>
       </c>
       <c r="E22">
-        <v>105.0085084589653</v>
+        <v>105.0073865329499</v>
       </c>
       <c r="F22" t="s">
         <v>77</v>
@@ -4329,13 +4419,13 @@
         <v>0</v>
       </c>
       <c r="C23">
-        <v>104.3680632499619</v>
+        <v>104.3680632499615</v>
       </c>
       <c r="D23">
-        <v>104.3696498437788</v>
+        <v>104.3707000383894</v>
       </c>
       <c r="E23">
-        <v>104.3664766561451</v>
+        <v>104.3654264615336</v>
       </c>
       <c r="F23" t="s">
         <v>78</v>
@@ -4490,13 +4580,13 @@
         <v>0</v>
       </c>
       <c r="C24">
-        <v>104.3126919353054</v>
+        <v>104.3126919353048</v>
       </c>
       <c r="D24">
-        <v>104.3145780985553</v>
+        <v>104.3155202081765</v>
       </c>
       <c r="E24">
-        <v>104.3108057720555</v>
+        <v>104.3098636624332</v>
       </c>
       <c r="F24" t="s">
         <v>79</v>
@@ -4651,13 +4741,13 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <v>104.2257295771521</v>
+        <v>104.2257295771513</v>
       </c>
       <c r="D25">
-        <v>104.2273165463451</v>
+        <v>104.2283695796335</v>
       </c>
       <c r="E25">
-        <v>104.224142607959</v>
+        <v>104.2230895746691</v>
       </c>
       <c r="F25" t="s">
         <v>80</v>
@@ -4812,13 +4902,13 @@
         <v>0</v>
       </c>
       <c r="C26">
-        <v>104.1960993292178</v>
+        <v>104.1960993292168</v>
       </c>
       <c r="D26">
-        <v>104.1976191468289</v>
+        <v>104.1986981605256</v>
       </c>
       <c r="E26">
-        <v>104.1945795116067</v>
+        <v>104.1935004979079</v>
       </c>
       <c r="F26" t="s">
         <v>81</v>
@@ -4973,13 +5063,13 @@
         <v>0</v>
       </c>
       <c r="C27">
-        <v>104.1704620463554</v>
+        <v>104.1704620463543</v>
       </c>
       <c r="D27">
-        <v>104.1719472469835</v>
+        <v>104.1730377341506</v>
       </c>
       <c r="E27">
-        <v>104.1689768457274</v>
+        <v>104.167886358558</v>
       </c>
       <c r="F27" t="s">
         <v>82</v>
@@ -5134,13 +5224,13 @@
         <v>0</v>
       </c>
       <c r="C28">
-        <v>104.1304760563587</v>
+        <v>104.1304760563574</v>
       </c>
       <c r="D28">
-        <v>104.1321057842253</v>
+        <v>104.1331370802002</v>
       </c>
       <c r="E28">
-        <v>104.1288463284921</v>
+        <v>104.1278150325146</v>
       </c>
       <c r="F28" t="s">
         <v>83</v>
@@ -5304,13 +5394,13 @@
         <v>0</v>
       </c>
       <c r="C29">
-        <v>104.0881823033902</v>
+        <v>104.0881823033887</v>
       </c>
       <c r="D29">
-        <v>104.0898673035353</v>
+        <v>104.0908765443104</v>
       </c>
       <c r="E29">
-        <v>104.0864973032451</v>
+        <v>104.085488062467</v>
       </c>
       <c r="F29" t="s">
         <v>84</v>
@@ -5474,13 +5564,13 @@
         <v>0</v>
       </c>
       <c r="C30">
-        <v>104.0231235569988</v>
+        <v>104.0231235569971</v>
       </c>
       <c r="D30">
-        <v>104.0245676588451</v>
+        <v>104.0256754807602</v>
       </c>
       <c r="E30">
-        <v>104.0216794551525</v>
+        <v>104.0205716332341</v>
       </c>
       <c r="F30" t="s">
         <v>85</v>
@@ -5644,13 +5734,13 @@
         <v>0</v>
       </c>
       <c r="C31">
-        <v>103.9344078217967</v>
+        <v>103.9344078217949</v>
       </c>
       <c r="D31">
-        <v>103.9356973479207</v>
+        <v>103.9368727146157</v>
       </c>
       <c r="E31">
-        <v>103.9331182956726</v>
+        <v>103.931942928974</v>
       </c>
       <c r="F31" t="s">
         <v>86</v>
@@ -5805,13 +5895,13 @@
         <v>0</v>
       </c>
       <c r="C32">
-        <v>103.8276309054933</v>
+        <v>103.8276309054913</v>
       </c>
       <c r="D32">
-        <v>103.829385227669</v>
+        <v>103.8303675004223</v>
       </c>
       <c r="E32">
-        <v>103.8258765833175</v>
+        <v>103.8248943105603</v>
       </c>
       <c r="F32" t="s">
         <v>87</v>
@@ -5966,13 +6056,13 @@
         <v>0</v>
       </c>
       <c r="C33">
-        <v>104.9489164406664</v>
+        <v>104.9489164406672</v>
       </c>
       <c r="D33">
-        <v>104.9507036265501</v>
+        <v>104.9516906151445</v>
       </c>
       <c r="E33">
-        <v>104.9471292547827</v>
+        <v>104.94614226619</v>
       </c>
       <c r="F33" t="s">
         <v>88</v>
@@ -6136,13 +6226,13 @@
         <v>0</v>
       </c>
       <c r="C34">
-        <v>103.7308830678859</v>
+        <v>103.7308830678838</v>
       </c>
       <c r="D34">
-        <v>103.7330620423747</v>
+        <v>103.7339074430993</v>
       </c>
       <c r="E34">
-        <v>103.7287040933972</v>
+        <v>103.7278586926683</v>
       </c>
       <c r="F34" t="s">
         <v>89</v>
@@ -6297,13 +6387,13 @@
         <v>0</v>
       </c>
       <c r="C35">
-        <v>103.6624578760893</v>
+        <v>103.6624578760871</v>
       </c>
       <c r="D35">
-        <v>103.6652135121418</v>
+        <v>103.6659214122869</v>
       </c>
       <c r="E35">
-        <v>103.6597022400369</v>
+        <v>103.6589943398873</v>
       </c>
       <c r="F35" t="s">
         <v>90</v>
@@ -6467,13 +6557,13 @@
         <v>0</v>
       </c>
       <c r="C36">
-        <v>103.6087907623864</v>
+        <v>103.608790762384</v>
       </c>
       <c r="D36">
-        <v>103.6114036204602</v>
+        <v>103.6121411986883</v>
       </c>
       <c r="E36">
-        <v>103.6061779043126</v>
+        <v>103.6054403260797</v>
       </c>
       <c r="F36" t="s">
         <v>91</v>
@@ -6628,13 +6718,13 @@
         <v>0</v>
       </c>
       <c r="C37">
-        <v>103.5659914634114</v>
+        <v>103.565991463409</v>
       </c>
       <c r="D37">
-        <v>103.5684926233496</v>
+        <v>103.5692570743031</v>
       </c>
       <c r="E37">
-        <v>103.5634903034731</v>
+        <v>103.5627258525149</v>
       </c>
       <c r="F37" t="s">
         <v>92</v>
@@ -6789,13 +6879,13 @@
         <v>0</v>
       </c>
       <c r="C38">
-        <v>103.5172696587305</v>
+        <v>103.5172696587281</v>
       </c>
       <c r="D38">
-        <v>103.5201574264639</v>
+        <v>103.5208384226691</v>
       </c>
       <c r="E38">
-        <v>103.5143818909971</v>
+        <v>103.513700894787</v>
       </c>
       <c r="F38" t="s">
         <v>93</v>
@@ -6959,13 +7049,13 @@
         <v>0</v>
       </c>
       <c r="C39">
-        <v>103.4887754149115</v>
+        <v>103.488775414909</v>
       </c>
       <c r="D39">
-        <v>103.491610402942</v>
+        <v>103.4923014748131</v>
       </c>
       <c r="E39">
-        <v>103.4859404268809</v>
+        <v>103.485249355005</v>
       </c>
       <c r="F39" t="s">
         <v>94</v>
@@ -7129,13 +7219,13 @@
         <v>0</v>
       </c>
       <c r="C40">
-        <v>103.4559055051182</v>
+        <v>103.4559055051158</v>
       </c>
       <c r="D40">
-        <v>103.4562453462427</v>
+        <v>103.4580265539989</v>
       </c>
       <c r="E40">
-        <v>103.4555656639937</v>
+        <v>103.4537844562327</v>
       </c>
       <c r="F40" t="s">
         <v>95</v>
@@ -7287,13 +7377,13 @@
         <v>0</v>
       </c>
       <c r="C41">
-        <v>103.4278902320298</v>
+        <v>103.4278902320274</v>
       </c>
       <c r="D41">
-        <v>103.4303053887957</v>
+        <v>103.4310891685593</v>
       </c>
       <c r="E41">
-        <v>103.425475075264</v>
+        <v>103.4246912954955</v>
       </c>
       <c r="F41" t="s">
         <v>96</v>
@@ -7457,13 +7547,13 @@
         <v>0</v>
       </c>
       <c r="C42">
-        <v>103.3331921536596</v>
+        <v>103.3331921536572</v>
       </c>
       <c r="D42">
-        <v>103.3348172402021</v>
+        <v>103.3358421509222</v>
       </c>
       <c r="E42">
-        <v>103.331567067117</v>
+        <v>103.3305421563922</v>
       </c>
       <c r="F42" t="s">
         <v>97</v>
@@ -7618,13 +7708,13 @@
         <v>0</v>
       </c>
       <c r="C43">
-        <v>103.2528444567445</v>
+        <v>103.2528444567423</v>
       </c>
       <c r="D43">
-        <v>103.2541758749533</v>
+        <v>103.2553303313863</v>
       </c>
       <c r="E43">
-        <v>103.2515130385356</v>
+        <v>103.2503585820984</v>
       </c>
       <c r="F43" t="s">
         <v>98</v>
@@ -7779,13 +7869,13 @@
         <v>0</v>
       </c>
       <c r="C44">
-        <v>104.8639764186466</v>
+        <v>104.8639764186472</v>
       </c>
       <c r="D44">
-        <v>104.8656316430069</v>
+        <v>104.8666700542124</v>
       </c>
       <c r="E44">
-        <v>104.8623211942863</v>
+        <v>104.8612827830819</v>
       </c>
       <c r="F44" t="s">
         <v>99</v>
@@ -7940,13 +8030,13 @@
         <v>0</v>
       </c>
       <c r="C45">
-        <v>103.1878120444685</v>
+        <v>103.1878120444667</v>
       </c>
       <c r="D45">
-        <v>103.1893041262504</v>
+        <v>103.1903849417755</v>
       </c>
       <c r="E45">
-        <v>103.1863199626867</v>
+        <v>103.1852391471579</v>
       </c>
       <c r="F45" t="s">
         <v>100</v>
@@ -8101,13 +8191,13 @@
         <v>0</v>
       </c>
       <c r="C46">
-        <v>103.0819243879698</v>
+        <v>103.0819243879684</v>
       </c>
       <c r="D46">
-        <v>103.0822356828407</v>
+        <v>103.0840410931364</v>
       </c>
       <c r="E46">
-        <v>103.0816130930989</v>
+        <v>103.0798076828004</v>
       </c>
       <c r="F46" t="s">
         <v>101</v>
@@ -8259,13 +8349,13 @@
         <v>0</v>
       </c>
       <c r="C47">
-        <v>103.0405382077004</v>
+        <v>103.0405382076992</v>
       </c>
       <c r="D47">
-        <v>103.0408186965253</v>
+        <v>103.0426544904364</v>
       </c>
       <c r="E47">
-        <v>103.0402577188755</v>
+        <v>103.038421924962</v>
       </c>
       <c r="F47" t="s">
         <v>102</v>
@@ -8417,13 +8507,13 @@
         <v>0</v>
       </c>
       <c r="C48">
-        <v>103.0144365300338</v>
+        <v>103.0144365300329</v>
       </c>
       <c r="D48">
-        <v>103.0156658274052</v>
+        <v>103.0168697233589</v>
       </c>
       <c r="E48">
-        <v>103.0132072326625</v>
+        <v>103.0120033367069</v>
       </c>
       <c r="F48" t="s">
         <v>103</v>
@@ -8578,13 +8668,13 @@
         <v>0</v>
       </c>
       <c r="C49">
-        <v>102.9828419847447</v>
+        <v>102.9828419847441</v>
       </c>
       <c r="D49">
-        <v>102.9843348641123</v>
+        <v>102.9854134450974</v>
       </c>
       <c r="E49">
-        <v>102.9813491053771</v>
+        <v>102.9802705243909</v>
       </c>
       <c r="F49" t="s">
         <v>104</v>
@@ -8739,13 +8829,13 @@
         <v>0</v>
       </c>
       <c r="C50">
-        <v>102.9481702855952</v>
+        <v>102.9481702855948</v>
       </c>
       <c r="D50">
-        <v>102.9495049034132</v>
+        <v>102.9506540365314</v>
       </c>
       <c r="E50">
-        <v>102.9468356677773</v>
+        <v>102.9456865346583</v>
       </c>
       <c r="F50" t="s">
         <v>105</v>
@@ -8903,10 +8993,10 @@
         <v>102.9217785963558</v>
       </c>
       <c r="D51">
-        <v>102.9233542119557</v>
+        <v>102.9244020489267</v>
       </c>
       <c r="E51">
-        <v>102.920202980756</v>
+        <v>102.9191551437849</v>
       </c>
       <c r="F51" t="s">
         <v>106</v>
@@ -9061,13 +9151,13 @@
         <v>0</v>
       </c>
       <c r="C52">
-        <v>102.8965797633679</v>
+        <v>102.8965797633683</v>
       </c>
       <c r="D52">
-        <v>102.8985455928063</v>
+        <v>102.8994546079718</v>
       </c>
       <c r="E52">
-        <v>102.8946139339295</v>
+        <v>102.8937049187648</v>
       </c>
       <c r="F52" t="s">
         <v>107</v>
@@ -9231,13 +9321,13 @@
         <v>0</v>
       </c>
       <c r="C53">
-        <v>102.8738679284233</v>
+        <v>102.873867928424</v>
       </c>
       <c r="D53">
-        <v>102.8754009734063</v>
+        <v>102.8764622801405</v>
       </c>
       <c r="E53">
-        <v>102.8723348834403</v>
+        <v>102.8712735767076</v>
       </c>
       <c r="F53" t="s">
         <v>108</v>
@@ -9392,13 +9482,13 @@
         <v>0</v>
       </c>
       <c r="C54">
-        <v>104.7624412087688</v>
+        <v>104.7624412087692</v>
       </c>
       <c r="D54">
-        <v>104.7640309098426</v>
+        <v>104.7650914031174</v>
       </c>
       <c r="E54">
-        <v>104.7608515076949</v>
+        <v>104.759791014421</v>
       </c>
       <c r="F54" t="s">
         <v>109</v>
@@ -9553,13 +9643,13 @@
         <v>0</v>
       </c>
       <c r="C55">
-        <v>104.7113554786701</v>
+        <v>104.7113554786704</v>
       </c>
       <c r="D55">
-        <v>104.7129955547126</v>
+        <v>104.7140342225497</v>
       </c>
       <c r="E55">
-        <v>104.7097154026276</v>
+        <v>104.708676734791</v>
       </c>
       <c r="F55" t="s">
         <v>110</v>
@@ -9714,13 +9804,13 @@
         <v>0</v>
       </c>
       <c r="C56">
-        <v>104.6549130713423</v>
+        <v>104.6549130713425</v>
       </c>
       <c r="D56">
-        <v>104.6565281368467</v>
+        <v>104.6575728859719</v>
       </c>
       <c r="E56">
-        <v>104.6532980058379</v>
+        <v>104.652253256713</v>
       </c>
       <c r="F56" t="s">
         <v>111</v>
@@ -9875,13 +9965,13 @@
         <v>0</v>
       </c>
       <c r="C57">
-        <v>104.5902999920136</v>
+        <v>104.5902999920137</v>
       </c>
       <c r="D57">
-        <v>104.5920748200843</v>
+        <v>104.5930609065037</v>
       </c>
       <c r="E57">
-        <v>104.5885251639429</v>
+        <v>104.5875390775236</v>
       </c>
       <c r="F57" t="s">
         <v>112</v>
@@ -10045,13 +10135,13 @@
         <v>0</v>
       </c>
       <c r="C58">
-        <v>104.5038603783446</v>
+        <v>104.5038603783445</v>
       </c>
       <c r="D58">
-        <v>104.5056515273796</v>
+        <v>104.5066320988317</v>
       </c>
       <c r="E58">
-        <v>104.5020692293097</v>
+        <v>104.5010886578574</v>
       </c>
       <c r="F58" t="s">
         <v>113</v>
@@ -10215,13 +10305,13 @@
         <v>0</v>
       </c>
       <c r="C59">
-        <v>104.4464620901627</v>
+        <v>104.4464620901624</v>
       </c>
       <c r="D59">
-        <v>104.4482787022762</v>
+        <v>104.4492477878056</v>
       </c>
       <c r="E59">
-        <v>104.4446454780492</v>
+        <v>104.4436763925192</v>
       </c>
       <c r="F59" t="s">
         <v>114</v>

</xml_diff>